<commit_message>
refactor 4: KAF004B: Update xu ly
(cherry picked from commit 2df9520cbd89c9246938897df61aa18fe4144afa)
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF002_レコーダーイメージ申請_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF002_レコーダーイメージ申請_template.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.50.4\share\500_新構想開発\04_設計\60_UI設計\K_就業\KAF_申請\KAF002_打刻申請\二次\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A219C3DC-583B-42CC-A293-02367AE08FD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE4BFCA-7ABE-421B-99D2-CB00EF9C42F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="出張申請" sheetId="28" r:id="rId1"/>
+    <sheet name="レコーダーイメージ申請" sheetId="28" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_Fill" localSheetId="0" hidden="1">#REF!</definedName>
@@ -418,39 +418,33 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -459,6 +453,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2522,7 +2522,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="AB16" sqref="AB16"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="11.25"/>
@@ -2558,10 +2558,10 @@
     <row r="3" spans="1:12" ht="15" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="6"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
@@ -2572,10 +2572,10 @@
     <row r="4" spans="1:12" ht="15" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="42"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="40"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
@@ -2599,8 +2599,8 @@
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="44"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="42"/>
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
@@ -2613,8 +2613,8 @@
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="44"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
@@ -2627,8 +2627,8 @@
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="35"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="47"/>
       <c r="D8" s="14"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
@@ -2641,8 +2641,8 @@
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="35"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="47"/>
       <c r="D9" s="14"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
@@ -2669,16 +2669,16 @@
     </row>
     <row r="11" spans="1:12" ht="90" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="47"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="45"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="3.75" customHeight="1">
@@ -2711,16 +2711,16 @@
     </row>
     <row r="14" spans="1:12" ht="74.25" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="40"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="38"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" ht="3.75" customHeight="1">
@@ -2929,7 +2929,7 @@
     <row r="37" ht="15" customHeight="1"/>
     <row r="38" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
     <mergeCell ref="C3:F3"/>
@@ -2938,6 +2938,8 @@
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:K11"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
refactor 4: KAF002: Update in
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF002_レコーダーイメージ申請_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF002_レコーダーイメージ申請_template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.50.4\share\500_新構想開発\04_設計\60_UI設計\K_就業\KAF_申請\KAF002_打刻申請\二次\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE4BFCA-7ABE-421B-99D2-CB00EF9C42F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12060"/>
   </bookViews>
   <sheets>
     <sheet name="レコーダーイメージ申請" sheetId="28" r:id="rId1"/>
@@ -64,19 +63,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -97,7 +96,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -455,19 +454,19 @@
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
-    <cellStyle name="標準 10" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="標準 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="標準 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="標準 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="標準 3 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="標準 10" xfId="2"/>
+    <cellStyle name="標準 2" xfId="1"/>
+    <cellStyle name="標準 2 2" xfId="4"/>
+    <cellStyle name="標準 3" xfId="3"/>
+    <cellStyle name="標準 3 2 2" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -508,7 +507,7 @@
         <xdr:cNvPr id="37" name="APPORVAL1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{346E8419-C746-4C23-9E43-AC947EA7C16C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{346E8419-C746-4C23-9E43-AC947EA7C16C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -516,8 +515,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3162300" y="219075"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="2819400" y="219075"/>
+          <a:ext cx="555766" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -527,7 +526,7 @@
           <xdr:cNvPr id="38" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{004784C8-04F9-4C18-A74C-486EAA9757D9}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{004784C8-04F9-4C18-A74C-486EAA9757D9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -581,7 +580,7 @@
           <xdr:cNvPr id="39" name="直線コネクタ 38">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FB3C29F-0EE3-40A2-940A-0CA748768656}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FB3C29F-0EE3-40A2-940A-0CA748768656}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -621,7 +620,7 @@
           <xdr:cNvPr id="40" name="直線コネクタ 39">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0097CE3E-9F77-43A2-A466-EAF2D36D2670}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0097CE3E-9F77-43A2-A466-EAF2D36D2670}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -661,7 +660,7 @@
           <xdr:cNvPr id="41" name="NAME1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D17CF269-B450-41AE-975B-64715D855A65}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D17CF269-B450-41AE-975B-64715D855A65}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -699,13 +698,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -714,7 +716,7 @@
           <xdr:cNvPr id="42" name="STATUS1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09683018-A19A-4CF2-91F9-99DAF09518CE}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09683018-A19A-4CF2-91F9-99DAF09518CE}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -752,13 +754,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -767,7 +772,7 @@
           <xdr:cNvPr id="43" name="DATE1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7609FF67-889F-484A-BB96-780296005F6D}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7609FF67-889F-484A-BB96-780296005F6D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -805,13 +810,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -836,7 +844,7 @@
         <xdr:cNvPr id="44" name="APPORVAL2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB59FA8E-2B91-4471-B5C7-D295177B1B9F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB59FA8E-2B91-4471-B5C7-D295177B1B9F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -844,8 +852,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3778822" y="219075"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="3369247" y="219075"/>
+          <a:ext cx="555766" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -855,7 +863,7 @@
           <xdr:cNvPr id="45" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD783704-E270-49AB-BB9D-757ACF898E2D}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD783704-E270-49AB-BB9D-757ACF898E2D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -909,7 +917,7 @@
           <xdr:cNvPr id="46" name="直線コネクタ 45">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B97B5839-6F27-4750-8D91-32AC7A1019B0}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B97B5839-6F27-4750-8D91-32AC7A1019B0}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -949,7 +957,7 @@
           <xdr:cNvPr id="47" name="直線コネクタ 46">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D95D8011-FD0C-44CB-B642-C550D1603F38}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D95D8011-FD0C-44CB-B642-C550D1603F38}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -989,7 +997,7 @@
           <xdr:cNvPr id="48" name="NAME2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AA7893D-4F1F-4CE1-B1C6-C8768770B9CE}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AA7893D-4F1F-4CE1-B1C6-C8768770B9CE}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1027,13 +1035,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1042,7 +1053,7 @@
           <xdr:cNvPr id="49" name="STATUS2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72C09801-5016-48D2-8191-199D8AE034C1}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72C09801-5016-48D2-8191-199D8AE034C1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1080,13 +1091,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1095,7 +1109,7 @@
           <xdr:cNvPr id="50" name="DATE2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F270D281-40B2-4F0E-883A-D448CBE4FB58}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F270D281-40B2-4F0E-883A-D448CBE4FB58}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1133,13 +1147,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1164,7 +1181,7 @@
         <xdr:cNvPr id="51" name="APPORVAL3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2389047B-DCB4-42A1-98BA-231294586AA0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2389047B-DCB4-42A1-98BA-231294586AA0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1172,8 +1189,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4403390" y="219075"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="3927140" y="219075"/>
+          <a:ext cx="546241" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1183,7 +1200,7 @@
           <xdr:cNvPr id="52" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65C3B46F-F180-4ABD-A30B-044DF0618DA3}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65C3B46F-F180-4ABD-A30B-044DF0618DA3}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1237,7 +1254,7 @@
           <xdr:cNvPr id="53" name="直線コネクタ 52">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEA078E8-87C0-45FE-A05F-374361B9DDF3}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEA078E8-87C0-45FE-A05F-374361B9DDF3}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1277,7 +1294,7 @@
           <xdr:cNvPr id="54" name="直線コネクタ 53">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DA076D7-52F8-4AE6-AF06-CBBAB277E27E}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DA076D7-52F8-4AE6-AF06-CBBAB277E27E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1317,7 +1334,7 @@
           <xdr:cNvPr id="55" name="NAME3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76EFA8F3-7AEF-41BE-AD5D-8263E9E02015}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76EFA8F3-7AEF-41BE-AD5D-8263E9E02015}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1355,13 +1372,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1370,7 +1390,7 @@
           <xdr:cNvPr id="56" name="STATUS3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E52E1A5-B644-4413-8CC2-BEA75454F67C}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E52E1A5-B644-4413-8CC2-BEA75454F67C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1408,13 +1428,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1423,7 +1446,7 @@
           <xdr:cNvPr id="57" name="DATE3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CC715D2-1A0B-4C99-813A-8D5B0600D6C1}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CC715D2-1A0B-4C99-813A-8D5B0600D6C1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1461,13 +1484,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1492,7 +1518,7 @@
         <xdr:cNvPr id="58" name="APPORVAL4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98C067D9-6241-4AC7-AB01-4447B24B9E5B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98C067D9-6241-4AC7-AB01-4447B24B9E5B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1500,8 +1526,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5017073" y="219075"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="4474148" y="219075"/>
+          <a:ext cx="555766" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1511,7 +1537,7 @@
           <xdr:cNvPr id="59" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24CAAF47-7F18-45FE-9F28-86FAEFBDAC73}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24CAAF47-7F18-45FE-9F28-86FAEFBDAC73}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1565,7 +1591,7 @@
           <xdr:cNvPr id="60" name="直線コネクタ 59">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6ACF279-C767-4A88-AE33-9781A12F431D}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6ACF279-C767-4A88-AE33-9781A12F431D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1605,7 +1631,7 @@
           <xdr:cNvPr id="61" name="直線コネクタ 60">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59FA6664-C71C-4B43-8AF5-1F253A46980F}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59FA6664-C71C-4B43-8AF5-1F253A46980F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1645,7 +1671,7 @@
           <xdr:cNvPr id="62" name="NAME4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7B6DA5C-771A-445A-96E7-82E616A57C9D}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7B6DA5C-771A-445A-96E7-82E616A57C9D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1683,13 +1709,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1698,7 +1727,7 @@
           <xdr:cNvPr id="63" name="STATUS4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3025EFE-BCA6-42DA-B701-43907F28FF80}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3025EFE-BCA6-42DA-B701-43907F28FF80}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1736,13 +1765,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1751,7 +1783,7 @@
           <xdr:cNvPr id="64" name="DATE4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5981CB7-5C2B-4742-B87C-61EE0829F439}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5981CB7-5C2B-4742-B87C-61EE0829F439}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1789,13 +1821,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1820,7 +1855,7 @@
         <xdr:cNvPr id="100" name="APPORVAL5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50C0D411-C243-4C60-AB73-A7775DA95CBF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50C0D411-C243-4C60-AB73-A7775DA95CBF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1828,8 +1863,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5641641" y="209550"/>
-          <a:ext cx="612916" cy="522000"/>
+          <a:off x="5032041" y="209550"/>
+          <a:ext cx="546241" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1839,7 +1874,7 @@
           <xdr:cNvPr id="101" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F93DFC2-081C-451C-9D48-B1BC9867336D}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F93DFC2-081C-451C-9D48-B1BC9867336D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1893,7 +1928,7 @@
           <xdr:cNvPr id="102" name="直線コネクタ 101">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6800343-807F-4136-B02C-74FB1EB4AA8C}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6800343-807F-4136-B02C-74FB1EB4AA8C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1933,7 +1968,7 @@
           <xdr:cNvPr id="103" name="直線コネクタ 102">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFCAF572-2F84-4462-BA25-EF7D0BEBF77F}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFCAF572-2F84-4462-BA25-EF7D0BEBF77F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1973,7 +2008,7 @@
           <xdr:cNvPr id="104" name="NAME5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038CF922-D380-4DD6-89F8-750F8F359F55}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038CF922-D380-4DD6-89F8-750F8F359F55}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2011,13 +2046,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2026,7 +2064,7 @@
           <xdr:cNvPr id="105" name="STATUS5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{716FE351-54BE-4E8A-8A72-99C2A31655FF}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{716FE351-54BE-4E8A-8A72-99C2A31655FF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2064,13 +2102,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2079,7 +2120,7 @@
           <xdr:cNvPr id="106" name="DATE5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1C5DE7D-8443-409E-AD02-44CD8415E210}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1C5DE7D-8443-409E-AD02-44CD8415E210}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2117,13 +2158,16 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2518,23 +2562,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2184022B-8B52-4EAD-B846-0F9397241960}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="0.77734375" style="2" customWidth="1"/>
-    <col min="2" max="11" width="7.21875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="0.77734375" style="2" customWidth="1"/>
-    <col min="13" max="14" width="7.109375" style="2" customWidth="1"/>
-    <col min="15" max="15" width="8.88671875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="1.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="0.75" style="2" customWidth="1"/>
+    <col min="2" max="11" width="7.25" style="2" customWidth="1"/>
+    <col min="12" max="12" width="0.75" style="2" customWidth="1"/>
+    <col min="13" max="14" width="7.125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="1.375" style="2" customWidth="1"/>
     <col min="17" max="17" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="2.44140625" style="2"/>
+    <col min="18" max="16384" width="2.5" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1">

</xml_diff>

<commit_message>
refactor 4: KAF002: Update in: chieu cao cot ly do
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF002_レコーダーイメージ申請_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF002_レコーダーイメージ申請_template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.50.4\share\500_新構想開発\04_設計\60_UI設計\K_就業\KAF_申請\KAF002_打刻申請\二次\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5F6487-97C1-4BBB-A409-8369B798E14E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12060"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="レコーダーイメージ申請" sheetId="28" r:id="rId1"/>
@@ -63,19 +64,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -96,7 +97,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -462,11 +463,11 @@
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
-    <cellStyle name="標準 10" xfId="2"/>
-    <cellStyle name="標準 2" xfId="1"/>
-    <cellStyle name="標準 2 2" xfId="4"/>
-    <cellStyle name="標準 3" xfId="3"/>
-    <cellStyle name="標準 3 2 2" xfId="5"/>
+    <cellStyle name="標準 10" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="標準 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="標準 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="標準 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="標準 3 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -507,7 +508,7 @@
         <xdr:cNvPr id="37" name="APPORVAL1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{346E8419-C746-4C23-9E43-AC947EA7C16C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{346E8419-C746-4C23-9E43-AC947EA7C16C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -515,8 +516,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2819400" y="219075"/>
-          <a:ext cx="555766" cy="522000"/>
+          <a:off x="3162300" y="219075"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -526,7 +527,7 @@
           <xdr:cNvPr id="38" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{004784C8-04F9-4C18-A74C-486EAA9757D9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{004784C8-04F9-4C18-A74C-486EAA9757D9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -580,7 +581,7 @@
           <xdr:cNvPr id="39" name="直線コネクタ 38">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FB3C29F-0EE3-40A2-940A-0CA748768656}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FB3C29F-0EE3-40A2-940A-0CA748768656}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -620,7 +621,7 @@
           <xdr:cNvPr id="40" name="直線コネクタ 39">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0097CE3E-9F77-43A2-A466-EAF2D36D2670}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0097CE3E-9F77-43A2-A466-EAF2D36D2670}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -660,7 +661,7 @@
           <xdr:cNvPr id="41" name="NAME1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D17CF269-B450-41AE-975B-64715D855A65}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D17CF269-B450-41AE-975B-64715D855A65}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -716,7 +717,7 @@
           <xdr:cNvPr id="42" name="STATUS1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09683018-A19A-4CF2-91F9-99DAF09518CE}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09683018-A19A-4CF2-91F9-99DAF09518CE}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -772,7 +773,7 @@
           <xdr:cNvPr id="43" name="DATE1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7609FF67-889F-484A-BB96-780296005F6D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7609FF67-889F-484A-BB96-780296005F6D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -844,7 +845,7 @@
         <xdr:cNvPr id="44" name="APPORVAL2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB59FA8E-2B91-4471-B5C7-D295177B1B9F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB59FA8E-2B91-4471-B5C7-D295177B1B9F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -852,8 +853,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3369247" y="219075"/>
-          <a:ext cx="555766" cy="522000"/>
+          <a:off x="3778822" y="219075"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -863,7 +864,7 @@
           <xdr:cNvPr id="45" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD783704-E270-49AB-BB9D-757ACF898E2D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD783704-E270-49AB-BB9D-757ACF898E2D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -917,7 +918,7 @@
           <xdr:cNvPr id="46" name="直線コネクタ 45">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B97B5839-6F27-4750-8D91-32AC7A1019B0}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B97B5839-6F27-4750-8D91-32AC7A1019B0}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -957,7 +958,7 @@
           <xdr:cNvPr id="47" name="直線コネクタ 46">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D95D8011-FD0C-44CB-B642-C550D1603F38}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D95D8011-FD0C-44CB-B642-C550D1603F38}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -997,7 +998,7 @@
           <xdr:cNvPr id="48" name="NAME2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AA7893D-4F1F-4CE1-B1C6-C8768770B9CE}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AA7893D-4F1F-4CE1-B1C6-C8768770B9CE}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1053,7 +1054,7 @@
           <xdr:cNvPr id="49" name="STATUS2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72C09801-5016-48D2-8191-199D8AE034C1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72C09801-5016-48D2-8191-199D8AE034C1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1109,7 +1110,7 @@
           <xdr:cNvPr id="50" name="DATE2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F270D281-40B2-4F0E-883A-D448CBE4FB58}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F270D281-40B2-4F0E-883A-D448CBE4FB58}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1181,7 +1182,7 @@
         <xdr:cNvPr id="51" name="APPORVAL3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2389047B-DCB4-42A1-98BA-231294586AA0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2389047B-DCB4-42A1-98BA-231294586AA0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1189,8 +1190,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3927140" y="219075"/>
-          <a:ext cx="546241" cy="522000"/>
+          <a:off x="4403390" y="219075"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1200,7 +1201,7 @@
           <xdr:cNvPr id="52" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65C3B46F-F180-4ABD-A30B-044DF0618DA3}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65C3B46F-F180-4ABD-A30B-044DF0618DA3}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1254,7 +1255,7 @@
           <xdr:cNvPr id="53" name="直線コネクタ 52">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEA078E8-87C0-45FE-A05F-374361B9DDF3}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEA078E8-87C0-45FE-A05F-374361B9DDF3}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1294,7 +1295,7 @@
           <xdr:cNvPr id="54" name="直線コネクタ 53">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DA076D7-52F8-4AE6-AF06-CBBAB277E27E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DA076D7-52F8-4AE6-AF06-CBBAB277E27E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1334,7 +1335,7 @@
           <xdr:cNvPr id="55" name="NAME3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76EFA8F3-7AEF-41BE-AD5D-8263E9E02015}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76EFA8F3-7AEF-41BE-AD5D-8263E9E02015}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1390,7 +1391,7 @@
           <xdr:cNvPr id="56" name="STATUS3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E52E1A5-B644-4413-8CC2-BEA75454F67C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E52E1A5-B644-4413-8CC2-BEA75454F67C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1446,7 +1447,7 @@
           <xdr:cNvPr id="57" name="DATE3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CC715D2-1A0B-4C99-813A-8D5B0600D6C1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CC715D2-1A0B-4C99-813A-8D5B0600D6C1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1518,7 +1519,7 @@
         <xdr:cNvPr id="58" name="APPORVAL4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98C067D9-6241-4AC7-AB01-4447B24B9E5B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98C067D9-6241-4AC7-AB01-4447B24B9E5B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1526,8 +1527,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4474148" y="219075"/>
-          <a:ext cx="555766" cy="522000"/>
+          <a:off x="5017073" y="219075"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1537,7 +1538,7 @@
           <xdr:cNvPr id="59" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24CAAF47-7F18-45FE-9F28-86FAEFBDAC73}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24CAAF47-7F18-45FE-9F28-86FAEFBDAC73}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1591,7 +1592,7 @@
           <xdr:cNvPr id="60" name="直線コネクタ 59">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6ACF279-C767-4A88-AE33-9781A12F431D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6ACF279-C767-4A88-AE33-9781A12F431D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1631,7 +1632,7 @@
           <xdr:cNvPr id="61" name="直線コネクタ 60">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59FA6664-C71C-4B43-8AF5-1F253A46980F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59FA6664-C71C-4B43-8AF5-1F253A46980F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1671,7 +1672,7 @@
           <xdr:cNvPr id="62" name="NAME4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7B6DA5C-771A-445A-96E7-82E616A57C9D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7B6DA5C-771A-445A-96E7-82E616A57C9D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1727,7 +1728,7 @@
           <xdr:cNvPr id="63" name="STATUS4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3025EFE-BCA6-42DA-B701-43907F28FF80}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3025EFE-BCA6-42DA-B701-43907F28FF80}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1783,7 +1784,7 @@
           <xdr:cNvPr id="64" name="DATE4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5981CB7-5C2B-4742-B87C-61EE0829F439}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5981CB7-5C2B-4742-B87C-61EE0829F439}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1855,7 +1856,7 @@
         <xdr:cNvPr id="100" name="APPORVAL5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50C0D411-C243-4C60-AB73-A7775DA95CBF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50C0D411-C243-4C60-AB73-A7775DA95CBF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1863,8 +1864,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5032041" y="209550"/>
-          <a:ext cx="546241" cy="522000"/>
+          <a:off x="5641641" y="209550"/>
+          <a:ext cx="612916" cy="522000"/>
           <a:chOff x="3466089" y="214591"/>
           <a:chExt cx="612916" cy="522000"/>
         </a:xfrm>
@@ -1874,7 +1875,7 @@
           <xdr:cNvPr id="101" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F93DFC2-081C-451C-9D48-B1BC9867336D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F93DFC2-081C-451C-9D48-B1BC9867336D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1928,7 +1929,7 @@
           <xdr:cNvPr id="102" name="直線コネクタ 101">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6800343-807F-4136-B02C-74FB1EB4AA8C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6800343-807F-4136-B02C-74FB1EB4AA8C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1968,7 +1969,7 @@
           <xdr:cNvPr id="103" name="直線コネクタ 102">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFCAF572-2F84-4462-BA25-EF7D0BEBF77F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFCAF572-2F84-4462-BA25-EF7D0BEBF77F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2008,7 +2009,7 @@
           <xdr:cNvPr id="104" name="NAME5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038CF922-D380-4DD6-89F8-750F8F359F55}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038CF922-D380-4DD6-89F8-750F8F359F55}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2064,7 +2065,7 @@
           <xdr:cNvPr id="105" name="STATUS5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{716FE351-54BE-4E8A-8A72-99C2A31655FF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{716FE351-54BE-4E8A-8A72-99C2A31655FF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2120,7 +2121,7 @@
           <xdr:cNvPr id="106" name="DATE5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1C5DE7D-8443-409E-AD02-44CD8415E210}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1C5DE7D-8443-409E-AD02-44CD8415E210}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2562,21 +2563,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="0.75" style="2" customWidth="1"/>
-    <col min="2" max="11" width="7.25" style="2" customWidth="1"/>
-    <col min="12" max="12" width="0.75" style="2" customWidth="1"/>
-    <col min="13" max="14" width="7.125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="8.875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="1.375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="0.77734375" style="2" customWidth="1"/>
+    <col min="2" max="11" width="7.21875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="0.77734375" style="2" customWidth="1"/>
+    <col min="13" max="14" width="7.109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="1.33203125" style="2" customWidth="1"/>
     <col min="17" max="17" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="2.5" style="2"/>
+    <col min="18" max="16384" width="2.44140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1">
@@ -2709,7 +2712,7 @@
       <c r="K10" s="21"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" ht="90" customHeight="1">
+    <row r="11" spans="1:12" ht="93.75" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="34"/>
       <c r="C11" s="35"/>

</xml_diff>

<commit_message>
refactor 5: KAF000: Update function in theo bug 115671 115672 115673
(cherry picked from commit 353c91ff165790f61c52129ab71ca8f553c7a8ba)
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF002_レコーダーイメージ申請_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF002_レコーダーイメージ申請_template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.50.4\share\500_新構想開発\04_設計\60_UI設計\K_就業\KAF_申請\KAF002_打刻申請\二次\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02.Project\UK\nts.uk\uk.at\at.ctx\request\nts.uk.ctx.at.request.infra\src\main\resources\application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5F6487-97C1-4BBB-A409-8369B798E14E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="レコーダーイメージ申請" sheetId="28" r:id="rId1"/>
@@ -64,7 +63,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="12"/>
@@ -462,12 +461,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
-    <cellStyle name="標準 10" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="標準 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="標準 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="標準 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="標準 3 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準 10" xfId="2"/>
+    <cellStyle name="標準 2" xfId="1"/>
+    <cellStyle name="標準 2 2" xfId="4"/>
+    <cellStyle name="標準 3" xfId="3"/>
+    <cellStyle name="標準 3 2 2" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -508,7 +507,7 @@
         <xdr:cNvPr id="37" name="APPORVAL1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{346E8419-C746-4C23-9E43-AC947EA7C16C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{346E8419-C746-4C23-9E43-AC947EA7C16C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -527,7 +526,7 @@
           <xdr:cNvPr id="38" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{004784C8-04F9-4C18-A74C-486EAA9757D9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{004784C8-04F9-4C18-A74C-486EAA9757D9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -581,7 +580,7 @@
           <xdr:cNvPr id="39" name="直線コネクタ 38">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FB3C29F-0EE3-40A2-940A-0CA748768656}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3FB3C29F-0EE3-40A2-940A-0CA748768656}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -621,7 +620,7 @@
           <xdr:cNvPr id="40" name="直線コネクタ 39">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0097CE3E-9F77-43A2-A466-EAF2D36D2670}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0097CE3E-9F77-43A2-A466-EAF2D36D2670}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -661,7 +660,7 @@
           <xdr:cNvPr id="41" name="NAME1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D17CF269-B450-41AE-975B-64715D855A65}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D17CF269-B450-41AE-975B-64715D855A65}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -699,16 +698,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -717,7 +713,7 @@
           <xdr:cNvPr id="42" name="STATUS1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09683018-A19A-4CF2-91F9-99DAF09518CE}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{09683018-A19A-4CF2-91F9-99DAF09518CE}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -755,16 +751,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -773,7 +766,7 @@
           <xdr:cNvPr id="43" name="DATE1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7609FF67-889F-484A-BB96-780296005F6D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7609FF67-889F-484A-BB96-780296005F6D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -811,16 +804,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -845,7 +835,7 @@
         <xdr:cNvPr id="44" name="APPORVAL2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB59FA8E-2B91-4471-B5C7-D295177B1B9F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FB59FA8E-2B91-4471-B5C7-D295177B1B9F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -864,7 +854,7 @@
           <xdr:cNvPr id="45" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD783704-E270-49AB-BB9D-757ACF898E2D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AD783704-E270-49AB-BB9D-757ACF898E2D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -918,7 +908,7 @@
           <xdr:cNvPr id="46" name="直線コネクタ 45">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B97B5839-6F27-4750-8D91-32AC7A1019B0}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B97B5839-6F27-4750-8D91-32AC7A1019B0}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -958,7 +948,7 @@
           <xdr:cNvPr id="47" name="直線コネクタ 46">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D95D8011-FD0C-44CB-B642-C550D1603F38}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D95D8011-FD0C-44CB-B642-C550D1603F38}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -998,7 +988,7 @@
           <xdr:cNvPr id="48" name="NAME2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AA7893D-4F1F-4CE1-B1C6-C8768770B9CE}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8AA7893D-4F1F-4CE1-B1C6-C8768770B9CE}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1036,16 +1026,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1054,7 +1041,7 @@
           <xdr:cNvPr id="49" name="STATUS2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72C09801-5016-48D2-8191-199D8AE034C1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{72C09801-5016-48D2-8191-199D8AE034C1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1092,16 +1079,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1110,7 +1094,7 @@
           <xdr:cNvPr id="50" name="DATE2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F270D281-40B2-4F0E-883A-D448CBE4FB58}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F270D281-40B2-4F0E-883A-D448CBE4FB58}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1148,16 +1132,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1182,7 +1163,7 @@
         <xdr:cNvPr id="51" name="APPORVAL3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2389047B-DCB4-42A1-98BA-231294586AA0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2389047B-DCB4-42A1-98BA-231294586AA0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1201,7 +1182,7 @@
           <xdr:cNvPr id="52" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65C3B46F-F180-4ABD-A30B-044DF0618DA3}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{65C3B46F-F180-4ABD-A30B-044DF0618DA3}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1255,7 +1236,7 @@
           <xdr:cNvPr id="53" name="直線コネクタ 52">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEA078E8-87C0-45FE-A05F-374361B9DDF3}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CEA078E8-87C0-45FE-A05F-374361B9DDF3}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1295,7 +1276,7 @@
           <xdr:cNvPr id="54" name="直線コネクタ 53">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DA076D7-52F8-4AE6-AF06-CBBAB277E27E}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DA076D7-52F8-4AE6-AF06-CBBAB277E27E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1335,7 +1316,7 @@
           <xdr:cNvPr id="55" name="NAME3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76EFA8F3-7AEF-41BE-AD5D-8263E9E02015}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{76EFA8F3-7AEF-41BE-AD5D-8263E9E02015}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1373,16 +1354,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1391,7 +1369,7 @@
           <xdr:cNvPr id="56" name="STATUS3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E52E1A5-B644-4413-8CC2-BEA75454F67C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8E52E1A5-B644-4413-8CC2-BEA75454F67C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1429,16 +1407,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1447,7 +1422,7 @@
           <xdr:cNvPr id="57" name="DATE3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CC715D2-1A0B-4C99-813A-8D5B0600D6C1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8CC715D2-1A0B-4C99-813A-8D5B0600D6C1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1485,16 +1460,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1519,7 +1491,7 @@
         <xdr:cNvPr id="58" name="APPORVAL4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98C067D9-6241-4AC7-AB01-4447B24B9E5B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{98C067D9-6241-4AC7-AB01-4447B24B9E5B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1538,7 +1510,7 @@
           <xdr:cNvPr id="59" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24CAAF47-7F18-45FE-9F28-86FAEFBDAC73}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{24CAAF47-7F18-45FE-9F28-86FAEFBDAC73}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1592,7 +1564,7 @@
           <xdr:cNvPr id="60" name="直線コネクタ 59">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6ACF279-C767-4A88-AE33-9781A12F431D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E6ACF279-C767-4A88-AE33-9781A12F431D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1632,7 +1604,7 @@
           <xdr:cNvPr id="61" name="直線コネクタ 60">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59FA6664-C71C-4B43-8AF5-1F253A46980F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{59FA6664-C71C-4B43-8AF5-1F253A46980F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1672,7 +1644,7 @@
           <xdr:cNvPr id="62" name="NAME4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7B6DA5C-771A-445A-96E7-82E616A57C9D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E7B6DA5C-771A-445A-96E7-82E616A57C9D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1710,16 +1682,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1728,7 +1697,7 @@
           <xdr:cNvPr id="63" name="STATUS4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3025EFE-BCA6-42DA-B701-43907F28FF80}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D3025EFE-BCA6-42DA-B701-43907F28FF80}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1766,16 +1735,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1784,7 +1750,7 @@
           <xdr:cNvPr id="64" name="DATE4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5981CB7-5C2B-4742-B87C-61EE0829F439}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A5981CB7-5C2B-4742-B87C-61EE0829F439}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1822,16 +1788,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -1856,7 +1819,7 @@
         <xdr:cNvPr id="100" name="APPORVAL5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50C0D411-C243-4C60-AB73-A7775DA95CBF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{50C0D411-C243-4C60-AB73-A7775DA95CBF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1875,7 +1838,7 @@
           <xdr:cNvPr id="101" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F93DFC2-081C-451C-9D48-B1BC9867336D}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0F93DFC2-081C-451C-9D48-B1BC9867336D}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1929,7 +1892,7 @@
           <xdr:cNvPr id="102" name="直線コネクタ 101">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6800343-807F-4136-B02C-74FB1EB4AA8C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B6800343-807F-4136-B02C-74FB1EB4AA8C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1969,7 +1932,7 @@
           <xdr:cNvPr id="103" name="直線コネクタ 102">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFCAF572-2F84-4462-BA25-EF7D0BEBF77F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AFCAF572-2F84-4462-BA25-EF7D0BEBF77F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2009,7 +1972,7 @@
           <xdr:cNvPr id="104" name="NAME5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038CF922-D380-4DD6-89F8-750F8F359F55}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{038CF922-D380-4DD6-89F8-750F8F359F55}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2047,16 +2010,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2065,7 +2025,7 @@
           <xdr:cNvPr id="105" name="STATUS5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{716FE351-54BE-4E8A-8A72-99C2A31655FF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{716FE351-54BE-4E8A-8A72-99C2A31655FF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2103,16 +2063,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2121,7 +2078,7 @@
           <xdr:cNvPr id="106" name="DATE5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1C5DE7D-8443-409E-AD02-44CD8415E210}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D1C5DE7D-8443-409E-AD02-44CD8415E210}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2159,16 +2116,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="700">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+            </a:endParaRPr>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2563,12 +2517,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.44140625" defaultRowHeight="11.25"/>
   <cols>

</xml_diff>